<commit_message>
full size 100 db added
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5326d3c6001040d/Tiedostot/school/nlp/repository/nlp-text-categorization/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_B7DC49CD03E8150532219032AD529B5E1FC64909" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7892D5CA-4E4C-41B2-90FB-DFC4D02506C2}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mk" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,12 @@
     <sheet name="nm" sheetId="9" r:id="rId9"/>
     <sheet name="ch" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="247">
   <si>
     <t>title</t>
   </si>
@@ -52,6 +58,69 @@
     <t>Thickened synovium with a hypoxic oxygenation status as measured with                     photoacoustic imaging was associated with fewer Doppler US signals and higher                     disease activity in study participants with rheumatoid arthritis.</t>
   </si>
   <si>
+    <t>A Multicenter Randomized Controlled Study of Contrast-enhanced US                     versus US-guided Biopsy of Focal Liver Lesions</t>
+  </si>
+  <si>
+    <t>Wei Wu*,*,Xiang Jing*,*,Gai-qin Xue,Xiao-lin Zhu,Jing Wang,Rui-qing Du,Bin Lv,Ke-feng Wang,Ji-Ping Yan,Zhong-yi Zhang,Man-di Li,Yuko Kono,Kun Yan</t>
+  </si>
+  <si>
+    <t>Contrast-enhanced US-guided biopsy of focal liver lesions had a higher diagnostic                     accuracy than US-guided biopsy, especially for lesions smaller than 2 cm and for                     hepatocellular carcinoma diagnosis.</t>
+  </si>
+  <si>
+    <t>Deep Learning Detects Changes Indicative of Axial Spondyloarthritis                     at MRI of Sacroiliac Joints</t>
+  </si>
+  <si>
+    <t>Keno K. Bressem,Lisa C. Adams,Fabian Proft,Kay Geert A. Hermann,Torsten Diekhoff,Laura Spiller,Stefan M. Niehues,Marcus R. Makowski,Bernd Hamm,Mikhail Protopopov,Valeria Rios Rodriguez,Hildurn Haibel,Judith Rademacher,Murat Torgutalp,Robert G. Lambert,Xenofon Baraliakos,Walter P. Maksymowych,Janis L. Vahldiek*,*,Denis Poddubnyy*,*</t>
+  </si>
+  <si>
+    <t>A deep learning tool was able to detect active inflammatory and structural                     changes indicative of axial spondyloarthritis at MRI of sacroiliac joints.</t>
+  </si>
+  <si>
+    <t>Generalizability and Bias in a Deep Learning Pediatric Bone Age Prediction Model Using Hand Radiographs</t>
+  </si>
+  <si>
+    <t>Elham Beheshtian,Kristin Putman,Samantha M. Santomartino,Vishwa S. Parekh,Paul H. Yi</t>
+  </si>
+  <si>
+    <t>A deep learning bone age prediction model generalized well to an external test set but demonstrated clinically significant sex-, age-, and sexual maturity–based biases.</t>
+  </si>
+  <si>
+    <t>Openness and Transparency in the Evaluation of Bias in Artificial                     Intelligence</t>
+  </si>
+  <si>
+    <t>David B. Larson</t>
+  </si>
+  <si>
+    <t>err</t>
+  </si>
+  <si>
+    <t>Percutaneous Vertebroplasty for Pain Management in Malignant Fractures of the Spine with Epidural Involvement</t>
+  </si>
+  <si>
+    <t>Guillaume Saliou,El Moncef Kocheida,Pierre Lehmann,Claude Depriester,Gaëlle Paradot,Daniel Le Gars,Antonia Balut,Hervé Deramond</t>
+  </si>
+  <si>
+    <t>In the course of our study, we have been able to confirm the feasibility, efficiency, and safety of percutaneous vertebroplasty in the treatment of vertebral fractures of tumorous origin with epidural involvement, with or without neurologic symptoms of medullary or cauda equina compression.</t>
+  </si>
+  <si>
+    <t>Ultrashort Echo Time MR Imaging of Osteochondral Junction of the Knee at 3 T: Identification of Anatomic Structures Contributing to Signal Intensity</t>
+  </si>
+  <si>
+    <t>Won C. Bae,Jerry R. Dwek,Richard Znamirowski,Sheronda M. Statum,Juan C. Hermida,Darryl D. D’Lima,Robert L. Sah,Jiang Du,Christine B. Chung</t>
+  </si>
+  <si>
+    <t>Evaluation of ultrashort–echo time (UTE) MR imaging signal intensity patterns and identification of UTE signal sources may aid clinical assessment of the osteochondral junction and may provide new opportunities for assessing joint degeneration and repair.</t>
+  </si>
+  <si>
+    <t>CT of Sclerotic Bone Lesions: Imaging Features Differentiating Tuberous Sclerosis Complex with Lymphangioleiomyomatosis from Sporadic Lymphangioleiomymatosis</t>
+  </si>
+  <si>
+    <t>Nilo A. Avila,Andrew J. Dwyer,Antoinette Rabel,Thomas Darling,Chien-Hui Hong,Joel Moss</t>
+  </si>
+  <si>
+    <t>Sclerotic bone lesions evident at CT are more common and numerous in patients with tuberous sclerosis complex (TSC) or TSC with lymphangioleiomyomatosis (LAM) than in patients with sporadic LAM.</t>
+  </si>
+  <si>
     <t>Quantitative CT Evaluation of Small Pulmonary Vessels Has Functional                     and Prognostic Value in Pulmonary Hypertension</t>
   </si>
   <si>
@@ -70,6 +139,57 @@
     <t>In a prospective study, reduced lung function at hyperpolarized 129Xe                     MRI and extent of fibrotic structure at CT were associated with disease                     progression in idiopathic pulmonary fibrosis 1 year later.</t>
   </si>
   <si>
+    <t>CT Hyperdense Artery Sign and the Effect of Alteplase in Endovascular                     Thrombectomy after Acute Stroke</t>
+  </si>
+  <si>
+    <t>Yu Zhou*,*,Yantao Jing*,*,Johanna Ospel,Mayank Goyal,Rosalie McDonough,Xincan Yue,Yuwei Ren,Yan Sun,Biao Li,Wenkai Yu,Pengfei Yang,Yongwei Zhang,Lei Zhang,Zifu Li,Guoli Duan,Xiaofei Ye,Bo Hong,Huaizhang Shi,Hongxing Han,Shuai Li,Sheng Liu,Jianmin Liu,for the DIRECT-MT Investigators</t>
+  </si>
+  <si>
+    <t>After acute stroke, the hyperdense artery sign (HAS) at noncontrast CT indicated                     favorable clinical outcome to endovascular treatment plus alteplase, but adding                     alteplase seemed to indicate worse outcome without HAS.</t>
+  </si>
+  <si>
+    <t>Sex Differences in Airways at Chest CT: Results from the COPDGene                     Cohort</t>
+  </si>
+  <si>
+    <t>Surya P. Bhatt,Sandeep Bodduluri,Arie Nakhmani,Young-il Kim,Joseph M. Reinhardt,Eric A. Hoffman,Amin Motahari,Carla G. Wilson,Stephen M. Humphries,Elizabeth A. Regan,Dawn L. DeMeo</t>
+  </si>
+  <si>
+    <t>In never-smokers, airway lumen at chest CT images was smaller in women than men;                     in ever-smokers, worsening of lumen size impacted respiratory outcomes more in                     women than men.</t>
+  </si>
+  <si>
+    <t>Histopathologic Basis for a Chest CT Deep Learning Survival                     Prediction Model in Patients with Lung Adenocarcinoma</t>
+  </si>
+  <si>
+    <t>Ju Gang Nam,Samina Park,Chang Min Park,Yoon Kyung Jeon,Doo Hyun Chung,Jin Mo Goo,Young Tae Kim,Hyungjin Kim</t>
+  </si>
+  <si>
+    <t>Output from a preoperative chest CT-based deep learning model was associated with                     histopathologic risk factors of lung adenocarcinoma independent of the clinical                     T category and radiologic nodule type.</t>
+  </si>
+  <si>
+    <t>Relationship of Plaque Features at Coronary CT to Coronary                     Hemodynamics and Cardiovascular Events</t>
+  </si>
+  <si>
+    <t>Seokhun Yang*,*,Masahiro Hoshino*,*,Bon-Kwon Koo,Taishi Yonetsu,Jinlong Zhang,Doyeon Hwang,Eun-Seok Shin,Joon-Hyung Doh,Chang-Wook Nam,Jianan Wang,Shaoliang Chen,Nobuhiro Tanaka,Hitoshi Matsuo,Takashi Kubo,Hyuk-Jae Chang,Tsunekazu Kakuta,Jagat Narula</t>
+  </si>
+  <si>
+    <t>High-risk plaque features and plaque burden at coronary CT angiography were                     associated with cardiovascular events independent of coronary hemodynamic flow                     parameters.</t>
+  </si>
+  <si>
+    <t>Anemia Detection by Hemoglobin Quantification on Contrast-enhanced                     Photon-counting CT Data Sets</t>
+  </si>
+  <si>
+    <t>Josua A. Decker,Adrian Huber,Fevzi Senel,Stefanie Bette,Franziska Braun,Franka Risch,Piotr Woźnicki,Judith Becker,Daniel Popp,Mark Haerting,Bertram Jehs,Katharina Rippel,Claudia Wollny,Christian Scheurig-Muenkler,Thomas J. Kroencke,Florian Schwarz</t>
+  </si>
+  <si>
+    <t>Machine Learning for Adrenal Gland Segmentation and Classification of Normal and Adrenal Masses at CT</t>
+  </si>
+  <si>
+    <t>Cory Robinson-Weiss*,*,Jay Patel*,*,Bernardo C. Bizzo,Daniel I. Glazer,Christopher P. Bridge,Katherine P. Andriole,Borna Dabiri,John K. Chin,Keith Dreyer,Jayashree Kalpathy-Cramer**,**,William W. Mayo-Smith**,**</t>
+  </si>
+  <si>
+    <t>A machine learning algorithm was developed that can accurately segment and classify adrenal glands as normal or mass-containing on contrast-enhanced CT images, with performance similar to that of radiologists.</t>
+  </si>
+  <si>
     <t>Enhancement Type at Contrast-enhanced Mammography and Association                     with Malignancy</t>
   </si>
   <si>
@@ -85,7 +205,67 @@
     <t>Yan Chen,Jonathan J. James,Eleni Michalopoulou,Iain T. Darker,Jacquie Jenkins</t>
   </si>
   <si>
-    <t>err</t>
+    <t>Diffusion-weighted Breast MRI in Prediction of Upstaging in Women                     with Biopsy-proven Ductal Carcinoma in Situ</t>
+  </si>
+  <si>
+    <t>Shin Ae Lee*,*,Youkyoung Lee*,*,Han Suk Ryu,Myoung-jin Jang,Woo Kyung Moon,Hyeong-Gon Moon**,**,Su Hyun Lee**,**</t>
+  </si>
+  <si>
+    <t>Preoperative diffusion-weighted breast MRI together with clinical and pathologic                     factors identified women at high risk of upstaging to invasive cancer at initial                     breast surgery.</t>
+  </si>
+  <si>
+    <t>A Pilot Study to Assess the Performance of Phase-Sensitive Breast                     Tomosynthesis</t>
+  </si>
+  <si>
+    <t>Laurie L. Fajardo,Stephen L. Hillis,Bin Zheng,Molly Donovan Wong,Muhammad U. Ghani,Farid H. Omoumi,Yuhua Li,Peter Jenkins,Michael E. Peterson,Xizeng Wu,Hong Liu</t>
+  </si>
+  <si>
+    <t>In this pilot study for an inline phase-sensitive breast tomosynthesis (PBT)                     system, the true diagnostic performance of PBT was within 0.08 of the true                     diagnostic performance of standard digital breast tomosynthesis, with PBT having                     a 24% mean radiation dose reduction.</t>
+  </si>
+  <si>
+    <t>Association of Longitudinal Mammographic Breast Density Changes with                     Subsequent Breast Cancer Risk</t>
+  </si>
+  <si>
+    <t>Thi Xuan Mai Tran,Soyeoun Kim,Huiyeon Song,Eunhye Lee,Boyoung Park</t>
+  </si>
+  <si>
+    <t>In premenopausal and postmenopausal women undergoing three consecutive biennial                     mammographic screenings, a consecutive increase in breast density augmented                     future breast cancer risk whereas a continuous decrease was associated with a                     lower risk.</t>
+  </si>
+  <si>
+    <t>Prospective Evaluation of Ultrafast Breast MRI for Predicting Pathologic Response after Neoadjuvant Therapies</t>
+  </si>
+  <si>
+    <t>Toulsie Ramtohul,Clara Tescher,Pauline Vaflard,Joanna Cyrta,Noémie Girard,Caroline Malhaire,Anne Tardivon</t>
+  </si>
+  <si>
+    <t>The wash-in slope derived from initial ultrafast breast MRI may help predict pathologic complete response in participants with breast cancer treated with neoadjuvant therapies.</t>
+  </si>
+  <si>
+    <t>Background Parenchymal Enhancement at Postoperative Surveillance Breast MRI: Association with Future Second Breast Cancer Risk</t>
+  </si>
+  <si>
+    <t>Su Hyun Lee,Myoung-jin Jang,Heera Yoen,Youkyoung Lee,Yeon Soo Kim,Ah Reum Park,Su Min Ha,Soo-Yeon Kim,Jung Min Chang,Nariya Cho,Woo Kyung Moon</t>
+  </si>
+  <si>
+    <t>Background parenchymal enhancement assessed at postoperative surveillance breast MRI was independently associated with the future second breast cancer risk in women with a personal history of breast cancer.</t>
+  </si>
+  <si>
+    <t>Antithrombotic Therapy and Hematoma Risk during Image-guided                     Core-Needle Breast Biopsy</t>
+  </si>
+  <si>
+    <t>Vilert A. Loving,Brian S. Johnston,Denise H. Reddy,Leslie A. Welk,Hannah A. Lawther,Shayna C. Klein,Caroline M. Cranford,R. Christopher Reed,Pooja Rangan,Michael F. Morris</t>
+  </si>
+  <si>
+    <t>Because rates of clinically significant hematomas are low and did not differ                     between patients undergoing antithrombotic therapy and those not undergoing                     antithrombotic therapy, stopping antithrombotic therapy before image-guided core                     needle breast biopsies may be unnecessary.</t>
+  </si>
+  <si>
+    <t>The Digital Divide in Radiology: Computer Use for Health                     Care–related Tasks and Breast Cancer Screening</t>
+  </si>
+  <si>
+    <t>Peter Abraham,Patricia Balthazar,Nicholas James Reid,Efrén J. Flores,Anand K. Narayan</t>
+  </si>
+  <si>
+    <t>Reliance on digital patient portals and online scheduling may exacerbate existing                     health disparities in breast cancer screening.</t>
   </si>
   <si>
     <t>MRI Evaluation of Uterine Masses for Risk of Leiomyosarcoma: A                     Consensus Statement</t>
@@ -106,6 +286,60 @@
     <t>Hybrid multidimensional MRI had similar or improved reader performance, higher interobserver agreement, and faster interpretation time for a diversely experienced group of radiologists diagnosing clinically significant prostate cancer.</t>
   </si>
   <si>
+    <t>Comparison of Micro-US and Multiparametric MRI for Prostate Cancer                     Detection in Biopsy-Naive Men</t>
+  </si>
+  <si>
+    <t>Sangeet Ghai,Nathan Perlis,Chantal Atallah,Sarah Jokhu,Kateri Corr,Katherine Lajkosz,Peter F. Incze,Alexandre R. Zlotta,Umesh Jain,Hannah Fleming,Antonio Finelli,Theodorus H. van der Kwast*,*,Masoom A. Haider*,*</t>
+  </si>
+  <si>
+    <t>Multiparametric MRI and micro-US showed similar prostate cancer detection rates                     in biopsy-naive men; although micro-US was inferior to multiparametric MRI for                     biopsy avoidance, most MRI lesions were visible at micro-US.</t>
+  </si>
+  <si>
+    <t>Avoiding Unnecessary Biopsy after Multiparametric Prostate MRI with                     VERDICT Analysis: The INNOVATE Study</t>
+  </si>
+  <si>
+    <t>Saurabh Singh,Harriet Rogers,Baris Kanber,Joey Clemente,Hayley Pye,Edward W. Johnston,Tom Parry,Alistair Grey,Eoin Dinneen,Greg Shaw,Susan Heavey,Urszula Stopka-Farooqui,Aiman Haider,Alex Freeman,Francesco Giganti,David Atkinson,Caroline M. Moore,Hayley C. Whitaker,Daniel C. Alexander,Eleftheria Panagiotaki,Shonit Punwani</t>
+  </si>
+  <si>
+    <t>Fractional intracellular volume–derived Vascular, Extracellular, and                     Restricted Diffusion for Cytometry in Tumor analysis of multiparametric MRI                     findings resulted in better classification of clinically significant prostate                     cancer than did analysis of prostate-specific antigen density or lesion apparent                     diffusion coefficient.</t>
+  </si>
+  <si>
+    <t>Contribution of Dynamic Contrast-enhanced and Diffusion MRI to                     PI-RADS for Detecting Clinically Significant Prostate Cancer</t>
+  </si>
+  <si>
+    <t>Anoshirwan Andrej Tavakoli,Thomas Hielscher,Patrick Badura,Magdalena Görtz,Tristan Anselm Kuder,Regula Gnirs,Constantin Schwab,Markus Hohenfellner,Heinz-Peter Schlemmer,David Bonekamp</t>
+  </si>
+  <si>
+    <t>In multiparametric prostate MRI, dynamic contrast-enhancement parameters did not                     improve clinically significant prostate cancer prediction for apparent diffusion                     coefficient (ADC) PI-RADS score 3 peripheral zone lesions, whereas quantitative                     ADC measurement supported lesion upgrading.</t>
+  </si>
+  <si>
+    <t>Development and Validation of Multiparametric MRI–based                     Radiomics Models for Preoperative Risk Stratification of Endometrial                     Cancer</t>
+  </si>
+  <si>
+    <t>Thierry L. Lefebvre,Yoshiko Ueno,Anthony Dohan,Avishek Chatterjee,Martin Vallières,Eric Winter-Reinhold,Sameh Saif,Ives R. Levesque,Xing Ziggy Zeng,Reza Forghani,Jan Seuntjens,Philippe Soyer,Peter Savadjiev*,*,Caroline Reinhold*,*</t>
+  </si>
+  <si>
+    <t>Three-dimensional radiomics-based machine learning models can stratify women with                     endometrial carcinoma at preoperative multiparametric MRI based on high-risk                     histopathologic features and can identify advanced-stage cancer (International                     Federation of Gynecology and Obstetrics system) reproducibly across sets                     acquired at different centers.</t>
+  </si>
+  <si>
+    <t>MR Spectroscopy for Detecting Fumarate Hydratase Deficiency in Hereditary Leiomyomatosis and Renal Cell Carcinoma Syndrome</t>
+  </si>
+  <si>
+    <t>Guangyu Wu*,*,Guiqin Liu*,*,Jianfeng Wang,Shihang Pan,Yuansheng Luo,Yunze Xu,Wen Kong,Peng Sun,Jianrong Xu,Wei Xue,Jin Zhang</t>
+  </si>
+  <si>
+    <t>MR spectroscopy can depict fumarate accumulation in renal cancer related to fumarate hydratase deficiency in hereditary leiomyomatosis and renal cell carcinoma syndrome.</t>
+  </si>
+  <si>
+    <t>18F-DCFPyL PET/CT for Initially Diagnosed and                     Biochemically Recurrent Prostate Cancer: Prospective Trial with Pathologic                     Confirmation</t>
+  </si>
+  <si>
+    <t>Gary A. Ulaner,Beth Thomsen,Jeffrey Bassett,Robert Torrey,Craig Cox,Kevin Lin,Trushar Patel,Tust Techasith,Audrey Mauguen,Steven P. Rowe,Liza Lindenberg,Esther Mena,Peter Choyke,Jeffrey Yoshida</t>
+  </si>
+  <si>
+    <t>This prospective clinical trial demonstrated with histologic examination the high                     positive predictive value of                     2-(3-{1-carboxy-5-[(6-[(18)F]fluoro-pyridine-3-carbonyl)-amino]-pentyl}-ureido)-pentanedioic                     acid PET/CT for prostate cancer distant metastases and recurrences and                     identified sites of false-positive findings.</t>
+  </si>
+  <si>
     <t>CT-based Ballistic Wound Path Identification and Trajectory Analysis in Anatomic Ballistic Phantoms</t>
   </si>
   <si>
@@ -124,6 +358,66 @@
     <t>When lower extremity CT angiography was combined with whole-body CT imaging in a multiphasic protocol, important vascular injuries requiring surgical management were identified.</t>
   </si>
   <si>
+    <t>Outside Imaging in Emergency Department Transfer Patients: CD Import Reduces Rates of Subsequent Imaging Utilization</t>
+  </si>
+  <si>
+    <t>Aaron Sodickson,Jonathan Opraseuth,Stephen Ledbetter</t>
+  </si>
+  <si>
+    <t>Emergency department transfer patients with successful CD-ROM import had a 17% utilization decrease from 3.30 to 2.74 examinations per patient for all subsequent 24-hour imaging and a 16% decrease in 24-hour CT utilization from 1.41 to 1.19 scans per patient.</t>
+  </si>
+  <si>
+    <t>Hemorrhagic Shock in Polytrauma Patients: Early Detection with Renal Doppler Resistive Index Measurements</t>
+  </si>
+  <si>
+    <t>Francesco Corradi,Claudia Brusasco,Antonella Vezzani,Salvatore Palermo,Fiorella Altomonte,Paolo Moscatelli,Paolo Pelosi</t>
+  </si>
+  <si>
+    <t>Renal Doppler resistance index measurement may represent a clinically useful noninvasive method for early detection of occult hemorrhagic shock.</t>
+  </si>
+  <si>
+    <t>Acute Lower Intestinal Bleeding: Feasibility and Diagnostic Performance of CT Angiography</t>
+  </si>
+  <si>
+    <t>Milagros Martí,José M. Artigas,Gonzalo Garzón,Rodolfo Álvarez-Sala,Jorge A. Soto</t>
+  </si>
+  <si>
+    <t>In the majority of cases, we propose CT angiography as the first step in diagnostic evaluation of patients with substantial bleeding for confirmation of active or recent hemorrhage and correct identification of the site and cause of bleeding.</t>
+  </si>
+  <si>
+    <t>Acute Appendicitis on Abdominal MR Images: Training Readers to Improve Diagnostic Accuracy</t>
+  </si>
+  <si>
+    <t>Marjolein M. N. Leeuwenburgh,Bart M. Wiarda,Shandra Bipat,C. Yung Nio,Thomas L. Bollen,J. Joost Kardux,Sebastiaan Jensch,Patrick M. M. Bossuyt,Marja A. Boermeester,Jaap Stoker</t>
+  </si>
+  <si>
+    <t>Sensitivity of inexperienced readers in the evaluation of acute appendicitis on abdominal MR images improved after training with direct feedback.</t>
+  </si>
+  <si>
+    <t>Alternative Diagnoses to Suspected Appendicitis at CT</t>
+  </si>
+  <si>
+    <t>B. Dustin Pooler,Edward M. Lawrence1,1,Perry J. Pickhardt</t>
+  </si>
+  <si>
+    <t>CT frequently identifies an alternative cause for symptoms in adults clinically suspected of having acute appendicitis; these conditions often require hospitalization and invasive treatment, and diagnostic CT plays an instrumental role in the triage and treatment of these patients.</t>
+  </si>
+  <si>
+    <t>Head CT for Nontrauma Patients in the Emergency Department: Clinical Predictors of Abnormal Findings</t>
+  </si>
+  <si>
+    <t>Xi Wang,John J. You</t>
+  </si>
+  <si>
+    <t>This study identified several potential clinical predictors of abnormal head CT findings in emergency department patients who had not sustained trauma; prospective validation of a clinical prediction rule in this population is warranted.</t>
+  </si>
+  <si>
+    <t>Active Hemorrhage and Vascular Injuries in Splenic Trauma: Utility of the Arterial Phase in Multidetector CT</t>
+  </si>
+  <si>
+    <t>Jennifer W. Uyeda,Christina A. LeBedis,David R. Penn,Jorge A. Soto,Stephan W. Anderson</t>
+  </si>
+  <si>
     <t>Renal Inflammation: Targeted Iron Oxide Nanoparticles for Molecular MR Imaging in Mice</t>
   </si>
   <si>
@@ -142,6 +436,69 @@
     <t>The folate receptor (FR)-targeted ultrasmall superparamagnetic iron oxide P1133 showed a specific retention in various FR-positive human breast cancer cell lines in vitro and in an FR-positive human breast cancer xenograft model in vivo.</t>
   </si>
   <si>
+    <t>Allogeneic Renal Graft Rejection in a Rat Model: In Vivo MR Imaging of the Homing Trait of Macrophages</t>
+  </si>
+  <si>
+    <t>Eun Young Chae,Eun Ju Song,Jin Young Sohn,Sang-Tae Kim,Chul Woong Woo,Gyungyub Gong,Hee Jung Kang,Jin Seong Lee</t>
+  </si>
+  <si>
+    <t>The homing of intravenously administered superparamagnetic iron oxide–labeled macrophages can be monitored with MR imaging of the allograft rejection model.</t>
+  </si>
+  <si>
+    <t>Diffusion-weighted MR Imaging of Native and Transplanted Kidneys</t>
+  </si>
+  <si>
+    <t>Harriet C. Thoeny,Frederik De Keyzer</t>
+  </si>
+  <si>
+    <t>Diffusion-weighted MR imaging is a noninvasive imaging technique that is well suited for the work-up of focal and diffuse renal conditions and provides information one step beyond morphology.</t>
+  </si>
+  <si>
+    <t>Differential Gene Expression in Well-healed and Poorly Healed Experimental Aneurysms after Coil Treatment</t>
+  </si>
+  <si>
+    <t>Ramanathan Kadirvel,Yong-Hong Ding,Daying Dai,Debra A. Lewis,David F. Kallmes</t>
+  </si>
+  <si>
+    <t>Increased gene expression in densely packed aneurysms was associated with adhesion molecules, proteases, and cytokines in the rabbit aneurysm model; loosely packed aneurysms showed increased expression of multiple structural molecules, including collagens.</t>
+  </si>
+  <si>
+    <t>Recent Advances in Cytogenetics and Molecular Biology of Adult Hepatocellular Tumors: Implications for Imaging and Management</t>
+  </si>
+  <si>
+    <t>Alampady K. Shanbhogue,Srinivasa R. Prasad,Naoki Takahashi,Raghunandan Vikram,Dushyant V. Sahani</t>
+  </si>
+  <si>
+    <t>The role of multiphase multidetector CT and MR imaging in the detection, characterization, and staging of liver tumors, as well as in surveillance after a wide gamut of targeted treatments, continues to expand and evolve.</t>
+  </si>
+  <si>
+    <t>Global Trends in Hybrid Imaging</t>
+  </si>
+  <si>
+    <t>Hedvig Hricak,Byung Ihn Choi,Andrew M. Scott,Kazuro Sugimura,Ada Muellner,Gustav K. von Schulthess,Maximilian F. Reiser,Michael M. Graham,N. Reed Dunnick,Steven M. Larson</t>
+  </si>
+  <si>
+    <t>Because the use of PET/CT is growing more rapidly than that of any other hybrid imaging technique, it is particularly important for diagnostic radiologists and nuclear medicine physicians to establish new pathways of collaboration within institutions, nationally and internationally.</t>
+  </si>
+  <si>
+    <t>PET/CT Characteristics of Isolated Bone Metastases in Hepatocellular Carcinoma</t>
+  </si>
+  <si>
+    <t>Chi-Lai Ho,Sirong Chen,Thomas Kam Chau Cheng,Yim Lung Leung</t>
+  </si>
+  <si>
+    <t>Patients with isolated bone metastases are a subgroup of patients with hepatocellular carcinoma that exhibit a form of tracer characteristics different from and more frequent than that in the group of patients with metastases to bone and other organs.</t>
+  </si>
+  <si>
+    <t>Bimodal Thrombus Imaging: Simultaneous PET/MR Imaging with a Fibrin-targeted Dual PET/MR Probe—Feasibility Study in Rat Model</t>
+  </si>
+  <si>
+    <t>Ritika Uppal,Ciprian Catana,Ilknur Ay,Thomas Benner,A. Gregory Sorensen,Peter Caravan</t>
+  </si>
+  <si>
+    <t>The dual PET/MR fibrin-targeted probe clearly identified the thrombus with either modality.</t>
+  </si>
+  <si>
     <t>Elemental Imaging of Long-term Gadolinium Retention in Rodent                     Femur</t>
   </si>
   <si>
@@ -160,6 +517,69 @@
     <t>Through this effort, a national strategy to address overutilization should be developed as a reflection of the need for greater accountability by radiology and health care professions in general in their stewardship of the expensive technologies used to improve the health and health care of patients.</t>
   </si>
   <si>
+    <t>Method for Tracking Eye Gaze during Interpretation of Endoluminal 3D CT Colonography: Technical Description and Proposed Metrics for Analysis</t>
+  </si>
+  <si>
+    <t>Peter Phillips,Darren Boone,Susan Mallett,Stuart A. Taylor,Douglas G. Altman,David Manning,Alastair Gale,Steve Halligan</t>
+  </si>
+  <si>
+    <t>To investigate interpretation of modern three-dimensional medical image displays, we have developed a method for analyzing visual gaze when the abnormality is both moving and changing in size.</t>
+  </si>
+  <si>
+    <t>Overinterpretation and Misreporting of Diagnostic Accuracy Studies: Evidence of “Spin”</t>
+  </si>
+  <si>
+    <t>Eleanor A. Ochodo,Margriet C. de Haan,Johannes B. Reitsma,Lotty Hooft,Patrick M. Bossuyt,Mariska M. G. Leeflang</t>
+  </si>
+  <si>
+    <t>Approximately three in 10 studies of the diagnostic accuracy of biomarkers or other medical tests published in journals with an impact factor of 4 or higher show false-positive results, and almost all studies contain practices that facilitate overinterpretation.</t>
+  </si>
+  <si>
+    <t>Improving Consistency in Radiology Reporting through the Use of Department-wide Standardized Structured Reporting</t>
+  </si>
+  <si>
+    <t>David B. Larson,Alex J. Towbin,Rebecca M. Pryor,Lane F. Donnelly1,1</t>
+  </si>
+  <si>
+    <t>We found that it is possible to implement department-wide structured reporting with a high rate of adoption by radiologists.</t>
+  </si>
+  <si>
+    <t>Compliance with STARD Checklist among Studies of Coronary CT Angiography: Systematic Review</t>
+  </si>
+  <si>
+    <t>Stefan Walther,Sabine Schueler,Robert Tackmann,Georg M. Schuetz,Peter Schlattmann,Marc Dewey</t>
+  </si>
+  <si>
+    <t>Our study results show that the overall compliance with reporting guidelines of studies addressing the diagnostic accuracy of CT coronary angiography has improved over time and is moderate to good, with a higher total score for Standards for Reporting of Diagnostic Accuracy (STARD)-adopting journals than for non-STARD-adopting journals.</t>
+  </si>
+  <si>
+    <t>Iterative Reconstruction Algorithm for CT: Can Radiation Dose Be Decreased While Low-Contrast Detectability Is Preserved?</t>
+  </si>
+  <si>
+    <t>Sebastian T. Schindera,Devang Odedra,Syed Arsalan Raza,Tae Kyoung Kim,Hyun-Jung Jang,Zsolt Szucs-Farkas,Patrik Rogalla</t>
+  </si>
+  <si>
+    <t>Iterative reconstruction algorithms can mislead a radiologist in attempting to lower the patient’s radiation dose while maintaining the diagnostic effectiveness, as the new reconstruction technique substantially improves the quantitative image quality but not the diagnostic effectiveness.</t>
+  </si>
+  <si>
+    <t>Pediatric CT: Implementation of ASIR for Substantial Radiation Dose Reduction While Maintaining Pre-ASIR Image Noise</t>
+  </si>
+  <si>
+    <t>Samuel L. Brady,Bria M. Moore1,1,Brian S. Yee,Robert A. Kaufman</t>
+  </si>
+  <si>
+    <t>For a predominantly pediatric population imaged with 40% adaptive statistical iterative reconstruction, a mean radiation dose reduction of 39% (2.7/4.4 mGy; range, 23%–72%) was achieved in chest CT and a mean reduction of 29% (4.8/6.8 mGy; range, 20%–64%) was achieved in abdominopelvic CT with no change in image noise magnitude or contrast-to-noise ratio.</t>
+  </si>
+  <si>
+    <t>Association of Study Quality with Completeness of Reporting: Have Completeness of Reporting and Quality of Systematic Reviews and Meta-Analyses in Major Radiology Journals Changed Since Publication of the PRISMA Statement?</t>
+  </si>
+  <si>
+    <t>Adam S. Tunis,Matthew D. F. McInnes,Ramez Hanna,Kaisra Esmail</t>
+  </si>
+  <si>
+    <t>Completeness of reporting is associated with quality of systematic reviews and meta-analyses in major radiology journals with a few deficient areas; complete reporting has improved modestly since publication of the Preferred Reporting Items for Systematic Reviews and Meta-Analyses statement, and it is strongly correlated with study quality in these journals.</t>
+  </si>
+  <si>
     <t>Mock Trial at 2009 RSNA Annual Meeting: Jury Exonerates Radiologist for Failure to Communicate Abnormal Finding—But…</t>
   </si>
   <si>
@@ -178,6 +598,63 @@
     <t>By critiquing the strengths, weaknesses, and unique features of pertinent radiology Web sites, the goal of this article is to provide radiologists and trainees with a database of relevant Web sites relating to international and national organizations, patient information, and training.</t>
   </si>
   <si>
+    <t>The ABR and Resident Recall “Cheating”</t>
+  </si>
+  <si>
+    <t>Ferris M. Hall</t>
+  </si>
+  <si>
+    <t>In my opinion, the American Board of Radiology would best handle the current controversy by making previous examination questions, but not answers, publicly available.</t>
+  </si>
+  <si>
+    <t>Society of Abdominal Radiology Is Created by a Merger of the Society of Gastrointestinal Radiologists and the Society of Uroradiology: Form Follows Function</t>
+  </si>
+  <si>
+    <t>Stuart G. Silverman</t>
+  </si>
+  <si>
+    <t>I would like to share with the readership of Radiology the reasons why two respected and successful societies undertook this merger, explain how this new society will enhance and expand the missions of its parent organizations, and suggest why the specialty of radiology, regardless of subspecialty interests, will be better served.</t>
+  </si>
+  <si>
+    <t>Avoiding Testocracy</t>
+  </si>
+  <si>
+    <t>Richard B. Gunderman,Zachary Ballenger,Darel E. Heitkamp</t>
+  </si>
+  <si>
+    <t>We must be careful not to allow postgraduate education to degenerate into a testocracy, where board examinations so dominate learners’ and educators' perspectives that we lose sight of the real purpose of education.</t>
+  </si>
+  <si>
+    <t>ABR Examinations: The Why, What, and How</t>
+  </si>
+  <si>
+    <t>Gary J. Becker,Jennifer L. Bosma,Milton J. Guiberteau,Anthony M. Gerdeman,Donald P. Frush,James P. Borgstede,For the Board of Trustees of the American Board of Radiology</t>
+  </si>
+  <si>
+    <t>Standards developed over decades by experts using the scientific method should be the central feature in any discussion or critique of examinations given for the privilege of professional practice and for safeguarding the public well-being.</t>
+  </si>
+  <si>
+    <t>MR Imaging in Hypertrophic Cardiomyopathy: From Magnet to Bedside</t>
+  </si>
+  <si>
+    <t>Jan Bogaert,Iacopo Olivotto</t>
+  </si>
+  <si>
+    <t>Since its introduction in the mid-1980s, cardiac MR imaging has now evolved into a multiparametric imaging modality allowing a truly comprehensive patient- and disease-tailored appraisal of hypertrophic cardiomyopathy, providing information on major areas of interest including cardiac phenotype, its functional and hemodynamic characterization, presence and extent of microvascular dysfunction, and myocardial fibrosis.</t>
+  </si>
+  <si>
+    <t>The Interventional Radiology/Diagnostic Radiology Certificate: Asking                     the Hard Questions</t>
+  </si>
+  <si>
+    <t>Darel E. Heitkamp,Richard B. Gunderman</t>
+  </si>
+  <si>
+    <t>The Interventional Radiology/Diagnostic Radiology Certificate and                     Interventional Radiology Residency</t>
+  </si>
+  <si>
+    <t>John A. Kaufman</t>
+  </si>
+  <si>
     <t>177Lu–Prostate-specific Membrane Antigen                     Radioligand Therapy in Patients with Metastatic Castration-resistant Prostate                     Cancer</t>
   </si>
   <si>
@@ -194,13 +671,112 @@
   </si>
   <si>
     <t>Fluorocholine PET/CT changed the therapeutic care of 20% of patients at high risk for extracapsular extension.</t>
+  </si>
+  <si>
+    <t>Effect of Hepatic Steatosis on Liver FDG Uptake Measured in Mean Standard Uptake Values</t>
+  </si>
+  <si>
+    <t>Jonathan T. Abele,Christopher I. Fung</t>
+  </si>
+  <si>
+    <t>Hepatic steatosis does not appear to have any significant effect on fluorine 18 fluorodeoxyglucose uptake by the liver determined by using mean standardized uptake values.</t>
+  </si>
+  <si>
+    <t>Does Multidetector CT Attenuation Change in Colon Cancer Liver Metastases Treated with 90Y Help Predict Metabolic Activity at FDG PET?</t>
+  </si>
+  <si>
+    <t>Sandra M. Tochetto,Pedram Rezai,Maryam Rezvani,Paul Nikolaidis,Senta Berggruen,Bassel Atassi,Riad Salem,Vahid Yaghmai</t>
+  </si>
+  <si>
+    <t>The changes in multidetector CT attenuation correlate highly with the metabolic activity assessed by using FDG PET after 90Y treatment of colon cancer hepatic metastases.</t>
+  </si>
+  <si>
+    <t>Pediatric 99mTc-MDP Bone SPECT with Ordered Subset Expectation Maximization Iterative Reconstruction with Isotropic 3D Resolution Recovery</t>
+  </si>
+  <si>
+    <t>Eryn Caamano Stansfield,Niall Sheehy,David Zurakowski,A. Hans Vija,Frederic H. Fahey,S. Ted Treves</t>
+  </si>
+  <si>
+    <t>By using ordered subset expectation maximization with three-dimensional resolution recovery, improved image quality of technetium 99m methylene diphosphonate skeletal SPECT with either a 50% reduction in radiation dose, a 50% reduction in acquisition time, or a combination of both can be achieved.</t>
+  </si>
+  <si>
+    <t>Use of Laxative-augmented Contrast Medium in the Evaluation of Colorectal Foci at FDG PET</t>
+  </si>
+  <si>
+    <t>Yen-Kung Chen,Jui-Hao Chen,Chih-Cheng Tsui,Hsuan-Hung Chou,Ru-Hwa Cheng,Jainn-Shiun Chiu</t>
+  </si>
+  <si>
+    <t>Compared with a conventional PET or PET/CT imaging protocol, the use of laxative-augmented contrast medium and delayed PET/CT improved diagnostic accuracy and reduced the number of equivocal and false-positive findings in patients with colorectal FDG foci.</t>
+  </si>
+  <si>
+    <t>Real-time FDG PET Guidance during Biopsies and Radiofrequency Ablation Using Multimodality Fusion with Electromagnetic Navigation</t>
+  </si>
+  <si>
+    <t>Aradhana M. Venkatesan,Samuel Kadoury,Nadine Abi-Jaoudeh,Elliot B. Levy,Roberto Maass-Moreno,Jochen Krücker,Sandeep Dalal,Sheng Xu,Neil Glossop,Bradford J. Wood</t>
+  </si>
+  <si>
+    <t>Combined electromagnetic device tracking and CT/US/fluorine 18 fluorodeoxyglucose (FDG) PET fusion allows successful biopsy and ablation of lesions that either demonstrate heterogeneous FDG uptake or are not well seen or are totally inapparent at conventional diagnostic imaging.</t>
+  </si>
+  <si>
+    <t>Non–Small Cell Lung Cancer: Prognostic Importance of Positive FDG PET Findings in the Mediastinum for Patients with N0–N1 Disease at Pathologic Analysis</t>
+  </si>
+  <si>
+    <t>Liyi Xie,Mert Saynak,Nirmal K. Veeramachaneni,David V. Fried,Mandar R. Jagtap,Wing Keung Chiu,Daniel S. Higginson,Michael V. Lawrence,Amir H. Khandani,Bahjat F. Qaqish,Ronald C. Chen,Lawrence B. Marks</t>
+  </si>
+  <si>
+    <t>In non-small cell lung cancer, preoperative evaluation of the mediastinum with PET may complement the surgical and histologic findings.</t>
+  </si>
+  <si>
+    <t>Reduction in Radiation Dose in Mercaptoacetyltriglycerine Renography with Enhanced Planar Processing</t>
+  </si>
+  <si>
+    <t>Edward M. Hsiao,Xinhua Cao,David Zurakowski,Katherine A. Zukotynski,Laura A. Drubach,Frederick D. Grant,Amos Yahil,A. Hans Vija,Royal T. Davis,Frederic H. Fahey,S. Ted Treves</t>
+  </si>
+  <si>
+    <t>Reducing the dose of 99mTc-mercaptoacetyltriglycerine from 7.4 to 2.2 MBq/kg without noise reduction or from 7.4 to 1.5 MBq/kg with noise reduction did not compromise image quality; reducing it to 0.74 MBq/kg did not affect functional parameters.</t>
+  </si>
+  <si>
+    <t>Deep Learning Detection of Active Pulmonary Tuberculosis at Chest                     Radiography Matched the Clinical Performance of Radiologists</t>
+  </si>
+  <si>
+    <t>Sahar Kazemzadeh*,*,Jin Yu*,*,Shahar Jamshy,Rory Pilgrim,Zaid Nabulsi,Christina Chen,Neeral Beladia,Charles Lau,Scott Mayer McKinney,Thad Hughes,Atilla P. Kiraly,Sreenivasa Raju Kalidindi,Monde Muyoyeta,Jameson Malemela,Ting Shih,Greg S. Corrado,Lily Peng,Katherine Chou,Po-Hsuan Cameron Chen,Yun Liu,Krish Eswaran,Daniel Tse,Shravya Shetty**,**,Shruthi Prabhakara**,**</t>
+  </si>
+  <si>
+    <t>A deep learning system trained to detect active pulmonary tuberculosis using                     de-identified data from 10 countries had a clinical performance comparable to                     that of nine radiologists on test data sets.</t>
+  </si>
+  <si>
+    <t>Simplified Transfer Learning for Chest Radiography Models Using Less                     Data</t>
+  </si>
+  <si>
+    <t>Andrew B. Sellergren,Christina Chen,Zaid Nabulsi,Yuanzhen Li,Aaron Maschinot,Aaron Sarna,Jenny Huang,Charles Lau,Sreenivasa Raju Kalidindi,Mozziyar Etemadi,Florencia Garcia-Vicente,David Melnick,Yun Liu,Krish Eswaran,Daniel Tse,Neeral Beladia,Dilip Krishnan,Shravya Shetty</t>
+  </si>
+  <si>
+    <t>This method enabled prediction performance comparable to state-of-the-art deep                     learning models in multiple clinical tasks by using as few as 45 chest                     radiographs.</t>
+  </si>
+  <si>
+    <t>Visualization of the Associations between the CT Features Extracted                     from a Deep Learning Survival Prediction Model and Histopathologic Risk                     Factors</t>
+  </si>
+  <si>
+    <t>Masahiro Yanagawa</t>
+  </si>
+  <si>
+    <t>Prevalence and Long-term Outcomes of CT Interstitial Lung Abnormalities in a Health Screening Cohort</t>
+  </si>
+  <si>
+    <t>Jong Eun Lee*,*,Kum Ju Chae*,*,Young Ju Suh,Won Gi Jeong,Taebum Lee,Yun-Hyeon Kim,Gong Yong Jin,Yeon Joo Jeong1,1</t>
+  </si>
+  <si>
+    <t>Hyperpolarized Xenon MRI, Further Evidence of Its Use in Progressive                     Pulmonary Fibrosis?</t>
+  </si>
+  <si>
+    <t>Fergus Gleeson,Emily Fraser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +813,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -283,7 +867,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -315,9 +899,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -349,6 +951,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -524,14 +1144,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="151.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +1168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -553,7 +1179,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -562,6 +1188,83 @@
       </c>
       <c r="C3" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -570,14 +1273,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -588,26 +1291,103 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B8" t="s">
+        <v>242</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>245</v>
+      </c>
+      <c r="B10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -616,14 +1396,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="118.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="218.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -634,26 +1421,103 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -662,14 +1526,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="145.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="159.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -680,26 +1551,103 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -708,14 +1656,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="142.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -726,26 +1680,103 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -754,14 +1785,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="115.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="165.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -772,26 +1810,103 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -800,14 +1915,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -818,26 +1933,103 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -846,14 +2038,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -864,26 +2056,103 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>160</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -892,14 +2161,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -910,26 +2179,103 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>183</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>184</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -938,14 +2284,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -956,26 +2302,103 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>211</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>212</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" t="s">
+        <v>233</v>
+      </c>
+      <c r="C10" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>